<commit_message>
clarify we need details for all team members in contribution template
</commit_message>
<xml_diff>
--- a/workflow/MacaqueNet social behavioral data contribution template.xlsx
+++ b/workflow/MacaqueNet social behavioral data contribution template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/ms1042_exeter_ac_uk/Documents/Research Technician Stuff/Cayo Behavioural Stuff/database/workflow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1C52D99-E4B3-489B-B00B-D53B8B425880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{E1C52D99-E4B3-489B-B00B-D53B8B425880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2543A06-FCD5-4D69-B10D-B0E9C6CAFD87}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -217,28 +217,6 @@
   </si>
   <si>
     <t>e.g. 13 months</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve">data owner(s) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>(name, email, current affiliation)</t>
-    </r>
-  </si>
-  <si>
-    <t>e.g. Jane Doe (janedoe@gmail.com, Uni of Exeter); John Smith (johnsmith@gmail.com)</t>
   </si>
   <si>
     <r>
@@ -487,6 +465,22 @@
   </si>
   <si>
     <t>options: count (e.g. agonism), duration (e.g. grooming)</t>
+  </si>
+  <si>
+    <t>e.g. Jane Doe (janedoe@gmail.com, Uni of Exeter); John Smith (johnsmith@gmail.com, Arizona State University)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">data owner(s) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>(name, email, current affiliation of ALL team members associated with the dataset)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -848,7 +842,7 @@
   <dimension ref="A1:B1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -940,74 +934,74 @@
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4957,37 +4951,37 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>34</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C2" s="9">
         <v>36272</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F2" s="7">
         <v>12</v>
@@ -4995,35 +4989,35 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C3" s="9">
         <v>38687</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C4" s="9">
         <v>33637</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F4" s="7">
         <v>1</v>
@@ -5031,17 +5025,17 @@
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C5" s="9">
         <v>40830</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F5" s="7">
         <v>21</v>
@@ -5049,17 +5043,17 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C6" s="9">
         <v>37332</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F6" s="7">
         <v>30</v>
@@ -13037,126 +13031,126 @@
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D1" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>46</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>48</v>
       </c>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" s="7">
         <v>0</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C3" s="7">
         <v>0</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D4" s="7">
         <v>0</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E5" s="7">
         <v>0</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F6" s="7">
         <v>0</v>
@@ -13176,17 +13170,17 @@
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13194,23 +13188,23 @@
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14217,126 +14211,126 @@
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D1" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>46</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>48</v>
       </c>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" s="7">
         <v>0</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C3" s="7">
         <v>0</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D4" s="7">
         <v>0</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E5" s="7">
         <v>0</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F6" s="7">
         <v>0</v>
@@ -14356,17 +14350,17 @@
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -14374,23 +14368,23 @@
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -15397,126 +15391,126 @@
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15"/>
       <c r="B1" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D1" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>46</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>48</v>
       </c>
       <c r="G1" s="15"/>
       <c r="H1" s="15"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" s="15">
         <v>0</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C3" s="15">
         <v>0</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D4" s="15">
         <v>0</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E5" s="15">
         <v>0</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F6" s="15">
         <v>0</v>
@@ -15536,7 +15530,7 @@
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B8" s="18"/>
       <c r="C8" s="18"/>
@@ -15548,7 +15542,7 @@
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B9" s="18"/>
       <c r="C9" s="18"/>
@@ -15560,7 +15554,7 @@
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -15582,7 +15576,7 @@
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
@@ -15594,7 +15588,7 @@
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
@@ -15606,7 +15600,7 @@
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
@@ -15619,7 +15613,7 @@
     <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -16626,126 +16620,126 @@
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15"/>
       <c r="B1" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D1" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>46</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>48</v>
       </c>
       <c r="G1" s="15"/>
       <c r="H1" s="15"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" s="15">
         <v>0</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C3" s="15">
         <v>0</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D4" s="15">
         <v>0</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E5" s="15">
         <v>0</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F6" s="15">
         <v>0</v>
@@ -16765,7 +16759,7 @@
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B8" s="18"/>
       <c r="C8" s="18"/>
@@ -16777,7 +16771,7 @@
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B9" s="18"/>
       <c r="C9" s="18"/>
@@ -16789,7 +16783,7 @@
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -16811,7 +16805,7 @@
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
@@ -16823,7 +16817,7 @@
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
@@ -16835,7 +16829,7 @@
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
@@ -16848,7 +16842,7 @@
     <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>